<commit_message>
Add remaining jump opcodes
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CDE1B2-D00B-4BF4-9F91-2BE8FD7FC06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30507003-CD24-499A-BF07-9884C6CC6CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
@@ -1824,7 +1824,7 @@
   <dimension ref="B1:AK55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2673,7 +2673,7 @@
       <c r="S15" s="77"/>
       <c r="T15" s="12"/>
       <c r="W15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15" t="s">
         <v>91</v>
@@ -2734,7 +2734,7 @@
       <c r="S16" s="77"/>
       <c r="T16" s="12"/>
       <c r="W16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK16" t="s">
         <v>91</v>
@@ -2795,7 +2795,7 @@
       <c r="S17" s="77"/>
       <c r="T17" s="12"/>
       <c r="W17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK17" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Rename opcodes for better consistency
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30507003-CD24-499A-BF07-9884C6CC6CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E24C9-7B51-4AC8-8E0B-AEC5ACAB92E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -117,9 +117,6 @@
     <t>LDI</t>
   </si>
   <si>
-    <t>LDR</t>
-  </si>
-  <si>
     <t>rd</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>EXTENSION</t>
   </si>
   <si>
-    <t>STR</t>
-  </si>
-  <si>
     <t>Implemented</t>
   </si>
   <si>
@@ -529,6 +523,12 @@
   </si>
   <si>
     <t>Doesn't modify the stack</t>
+  </si>
+  <si>
+    <t>STA</t>
+  </si>
+  <si>
+    <t>LDA</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1437,6 +1437,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1823,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C23" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,10 +1865,10 @@
     </row>
     <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="31">
         <v>7</v>
@@ -1900,37 +1901,41 @@
         <v>13</v>
       </c>
       <c r="N3" s="58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R3" s="72" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S3" s="73" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="W3" s="29" t="s">
-        <v>73</v>
+        <v>82</v>
+      </c>
+      <c r="W3" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" s="97" t="str">
+        <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
+        <v>20/45</v>
       </c>
       <c r="AK3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -1960,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" s="62">
         <f>IF(L4="NA",1,2)</f>
@@ -1974,24 +1979,24 @@
         <v>0</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R4" s="74" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S4" s="75"/>
       <c r="T4" s="12"/>
       <c r="U4" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="W4" s="13">
+        <v>83</v>
+      </c>
+      <c r="W4" s="62">
         <v>1</v>
       </c>
       <c r="AK4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2024,7 +2029,7 @@
         <v>1</v>
       </c>
       <c r="L5" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M5" s="14">
         <f t="shared" ref="M5:M55" si="0">IF(L5="NA",1,2)</f>
@@ -2038,24 +2043,24 @@
         <v>0</v>
       </c>
       <c r="P5" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R5" s="76" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S5" s="77"/>
       <c r="T5" s="12"/>
       <c r="U5" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W5" s="14">
         <v>1</v>
       </c>
       <c r="AK5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2088,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M6" s="14">
         <f t="shared" si="0"/>
@@ -2102,24 +2107,24 @@
         <v>0</v>
       </c>
       <c r="P6" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R6" s="76" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S6" s="77"/>
       <c r="T6" s="12"/>
       <c r="U6" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W6" s="14">
         <v>1</v>
       </c>
       <c r="AK6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2152,7 +2157,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M7" s="14">
         <f t="shared" si="0"/>
@@ -2166,24 +2171,24 @@
         <v>0</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R7" s="76" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S7" s="77"/>
       <c r="T7" s="12"/>
       <c r="U7" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="W7" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2216,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M8" s="14">
         <f t="shared" si="0"/>
@@ -2230,24 +2235,24 @@
         <v>0</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q8" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R8" s="76" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S8" s="77"/>
       <c r="T8" s="12"/>
       <c r="U8" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W8" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2280,7 +2285,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="0"/>
@@ -2294,24 +2299,24 @@
         <v>0</v>
       </c>
       <c r="P9" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q9" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R9" s="76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S9" s="77"/>
       <c r="T9" s="12"/>
       <c r="U9" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="W9" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2344,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M10" s="14">
         <f t="shared" si="0"/>
@@ -2358,20 +2363,20 @@
         <v>0</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R10" s="76"/>
       <c r="S10" s="77"/>
       <c r="T10" s="12"/>
       <c r="U10" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W10" s="15"/>
       <c r="AK10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2404,7 +2409,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11" s="14">
         <f t="shared" si="0"/>
@@ -2418,25 +2423,25 @@
         <v>0</v>
       </c>
       <c r="P11" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R11" s="76"/>
       <c r="S11" s="77"/>
       <c r="T11" s="12"/>
       <c r="U11" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W11" s="15"/>
       <c r="AK11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>8</v>
@@ -2480,16 +2485,16 @@
         <v>8</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q12" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R12" s="76" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S12" s="77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T12" s="12"/>
       <c r="U12" s="64"/>
@@ -2497,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="AK12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2544,17 +2549,17 @@
         <v>8</v>
       </c>
       <c r="P13" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q13" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R13" s="76"/>
       <c r="S13" s="77"/>
       <c r="T13" s="12"/>
       <c r="W13" s="15"/>
       <c r="AK13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2601,13 +2606,13 @@
         <v>8</v>
       </c>
       <c r="P14" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q14" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R14" s="76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S14" s="77"/>
       <c r="T14" s="12"/>
@@ -2615,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="AK14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2662,13 +2667,13 @@
         <v>8</v>
       </c>
       <c r="P15" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q15" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R15" s="76" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S15" s="77"/>
       <c r="T15" s="12"/>
@@ -2676,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="AK15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2723,13 +2728,13 @@
         <v>8</v>
       </c>
       <c r="P16" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q16" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R16" s="76" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S16" s="77"/>
       <c r="T16" s="12"/>
@@ -2737,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="AK16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2784,13 +2789,13 @@
         <v>8</v>
       </c>
       <c r="P17" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q17" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R17" s="76" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S17" s="77"/>
       <c r="T17" s="12"/>
@@ -2798,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="AK17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2845,23 +2850,23 @@
         <v>8</v>
       </c>
       <c r="P18" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R18" s="76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="S18" s="77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T18" s="12"/>
       <c r="W18" s="14">
         <v>1</v>
       </c>
       <c r="AK18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2894,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M19" s="14">
         <f t="shared" si="0"/>
@@ -2908,28 +2913,28 @@
         <v>8</v>
       </c>
       <c r="P19" s="42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q19" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R19" s="76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="S19" s="77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T19" s="12"/>
       <c r="W19" s="14">
         <v>1</v>
       </c>
       <c r="AK19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="81" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>18</v>
@@ -2953,13 +2958,13 @@
         <v>0</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M20" s="14">
         <f t="shared" si="0"/>
@@ -2973,13 +2978,13 @@
         <v>10</v>
       </c>
       <c r="P20" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q20" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R20" s="76" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S20" s="77"/>
       <c r="T20" s="12"/>
@@ -2987,13 +2992,13 @@
         <v>1</v>
       </c>
       <c r="AK20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="81"/>
       <c r="C21" s="14" t="s">
-        <v>19</v>
+        <v>156</v>
       </c>
       <c r="D21" s="66">
         <v>0</v>
@@ -3014,10 +3019,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" s="56" t="s">
         <v>7</v>
@@ -3034,13 +3039,13 @@
         <v>10</v>
       </c>
       <c r="P21" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q21" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R21" s="76" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S21" s="77"/>
       <c r="T21" s="12"/>
@@ -3048,13 +3053,13 @@
         <v>1</v>
       </c>
       <c r="AK21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="81"/>
       <c r="C22" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="66">
         <v>0</v>
@@ -3075,13 +3080,13 @@
         <v>0</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M22" s="14">
         <f t="shared" si="0"/>
@@ -3095,13 +3100,13 @@
         <v>10</v>
       </c>
       <c r="P22" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q22" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R22" s="76" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S22" s="77"/>
       <c r="T22" s="12"/>
@@ -3109,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="AK22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3142,7 +3147,7 @@
         <v>4</v>
       </c>
       <c r="L23" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M23" s="14">
         <f t="shared" si="0"/>
@@ -3156,22 +3161,22 @@
         <v>10</v>
       </c>
       <c r="P23" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q23" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R23" s="76"/>
       <c r="S23" s="77"/>
       <c r="T23" s="12"/>
       <c r="W23" s="15"/>
       <c r="AK23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>4</v>
@@ -3201,7 +3206,7 @@
         <v>4</v>
       </c>
       <c r="L24" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M24" s="14">
         <f t="shared" si="0"/>
@@ -3215,23 +3220,23 @@
         <v>20</v>
       </c>
       <c r="P24" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q24" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R24" s="76"/>
       <c r="S24" s="77"/>
       <c r="T24" s="12"/>
       <c r="W24" s="15"/>
       <c r="AK24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="80"/>
       <c r="C25" s="14" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="D25" s="66">
         <v>0</v>
@@ -3252,10 +3257,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L25" s="56" t="s">
         <v>7</v>
@@ -3272,13 +3277,13 @@
         <v>20</v>
       </c>
       <c r="P25" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q25" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R25" s="76" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S25" s="77"/>
       <c r="T25" s="12"/>
@@ -3286,13 +3291,13 @@
         <v>1</v>
       </c>
       <c r="AK25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="80"/>
       <c r="C26" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="66">
         <v>0</v>
@@ -3313,13 +3318,13 @@
         <v>0</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L26" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M26" s="14">
         <f t="shared" si="0"/>
@@ -3333,13 +3338,13 @@
         <v>20</v>
       </c>
       <c r="P26" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q26" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R26" s="76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S26" s="77"/>
       <c r="T26" s="12"/>
@@ -3347,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="AK26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3380,7 +3385,7 @@
         <v>4</v>
       </c>
       <c r="L27" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M27" s="14">
         <f t="shared" si="0"/>
@@ -3394,25 +3399,25 @@
         <v>20</v>
       </c>
       <c r="P27" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q27" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R27" s="76"/>
       <c r="S27" s="77"/>
       <c r="T27" s="12"/>
       <c r="W27" s="15"/>
       <c r="AK27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="66">
         <v>0</v>
@@ -3427,19 +3432,19 @@
         <v>1</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L28" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M28" s="14">
         <f t="shared" si="0"/>
@@ -3453,13 +3458,13 @@
         <v>30</v>
       </c>
       <c r="P28" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q28" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R28" s="76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="S28" s="77"/>
       <c r="T28" s="12"/>
@@ -3467,15 +3472,15 @@
         <v>1</v>
       </c>
       <c r="AK28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="93" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="66">
         <v>0</v>
@@ -3496,13 +3501,13 @@
         <v>0</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L29" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M29" s="14">
         <f t="shared" si="0"/>
@@ -3516,29 +3521,29 @@
         <v>40</v>
       </c>
       <c r="P29" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q29" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R29" s="76" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="S29" s="77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="T29" s="12"/>
       <c r="W29" s="14">
         <v>1</v>
       </c>
       <c r="AK29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="93"/>
       <c r="C30" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="67">
         <v>0</v>
@@ -3559,10 +3564,10 @@
         <v>1</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L30" s="56" t="s">
         <v>7</v>
@@ -3579,29 +3584,29 @@
         <v>40</v>
       </c>
       <c r="P30" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q30" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R30" s="76" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S30" s="77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="T30" s="12"/>
       <c r="W30" s="14">
         <v>0</v>
       </c>
       <c r="AK30" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="93"/>
       <c r="C31" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="67">
         <v>0</v>
@@ -3622,13 +3627,13 @@
         <v>0</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M31" s="14">
         <f t="shared" si="0"/>
@@ -3642,29 +3647,29 @@
         <v>40</v>
       </c>
       <c r="P31" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q31" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R31" s="76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S31" s="77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T31" s="12"/>
       <c r="W31" s="14">
         <v>1</v>
       </c>
       <c r="AK31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="93"/>
       <c r="C32" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="67">
         <v>0</v>
@@ -3685,10 +3690,10 @@
         <v>1</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L32" s="56" t="s">
         <v>7</v>
@@ -3705,31 +3710,31 @@
         <v>40</v>
       </c>
       <c r="P32" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q32" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R32" s="76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S32" s="77" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="T32" s="12"/>
       <c r="W32" s="14">
         <v>0</v>
       </c>
       <c r="AK32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33" s="67">
         <v>0</v>
@@ -3744,19 +3749,19 @@
         <v>1</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L33" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M33" s="14">
         <f t="shared" si="0"/>
@@ -3770,29 +3775,29 @@
         <v>50</v>
       </c>
       <c r="P33" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q33" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R33" s="76" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S33" s="77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T33" s="12"/>
       <c r="W33" s="14">
         <v>0</v>
       </c>
       <c r="AK33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="94"/>
       <c r="C34" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="67">
         <v>0</v>
@@ -3807,19 +3812,19 @@
         <v>0</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L34" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M34" s="14">
         <f t="shared" si="0"/>
@@ -3833,31 +3838,31 @@
         <v>60</v>
       </c>
       <c r="P34" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q34" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R34" s="76" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S34" s="77" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="T34" s="12"/>
       <c r="W34" s="14">
         <v>0</v>
       </c>
       <c r="AK34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="95" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="67">
         <v>0</v>
@@ -3878,13 +3883,13 @@
         <v>0</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L35" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M35" s="14">
         <f t="shared" si="0"/>
@@ -3898,29 +3903,29 @@
         <v>70</v>
       </c>
       <c r="P35" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q35" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R35" s="76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="S35" s="77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T35" s="12"/>
       <c r="W35" s="14">
         <v>0</v>
       </c>
       <c r="AK35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="95"/>
       <c r="C36" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="67">
         <v>0</v>
@@ -3941,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L36" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M36" s="14">
         <f t="shared" si="0"/>
@@ -3961,29 +3966,29 @@
         <v>70</v>
       </c>
       <c r="P36" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q36" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R36" s="76" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S36" s="77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T36" s="12"/>
       <c r="W36" s="14">
         <v>0</v>
       </c>
       <c r="AK36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="95"/>
       <c r="C37" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D37" s="67">
         <v>0</v>
@@ -4004,13 +4009,13 @@
         <v>0</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L37" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M37" s="14">
         <f t="shared" si="0"/>
@@ -4024,29 +4029,29 @@
         <v>70</v>
       </c>
       <c r="P37" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q37" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R37" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="S37" s="77" t="s">
         <v>142</v>
-      </c>
-      <c r="S37" s="77" t="s">
-        <v>144</v>
       </c>
       <c r="T37" s="12"/>
       <c r="W37" s="14">
         <v>0</v>
       </c>
       <c r="AK37" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="95"/>
       <c r="C38" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="67">
         <v>0</v>
@@ -4067,13 +4072,13 @@
         <v>1</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L38" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M38" s="14">
         <f t="shared" si="0"/>
@@ -4087,31 +4092,31 @@
         <v>70</v>
       </c>
       <c r="P38" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q38" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R38" s="76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S38" s="77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="T38" s="12"/>
       <c r="W38" s="14">
         <v>0</v>
       </c>
       <c r="AK38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="96" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="67">
         <v>1</v>
@@ -4132,13 +4137,13 @@
         <v>0</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K39" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L39" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M39" s="14">
         <f t="shared" si="0"/>
@@ -4152,29 +4157,29 @@
         <v>80</v>
       </c>
       <c r="P39" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q39" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R39" s="76" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="S39" s="77" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T39" s="12"/>
       <c r="W39" s="14">
         <v>0</v>
       </c>
       <c r="AK39" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="96"/>
       <c r="C40" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="67">
         <v>1</v>
@@ -4195,10 +4200,10 @@
         <v>1</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L40" s="56" t="s">
         <v>7</v>
@@ -4215,29 +4220,29 @@
         <v>80</v>
       </c>
       <c r="P40" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q40" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R40" s="76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="S40" s="77" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T40" s="12"/>
       <c r="W40" s="14">
         <v>0</v>
       </c>
       <c r="AK40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="96"/>
       <c r="C41" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="67">
         <v>1</v>
@@ -4258,13 +4263,13 @@
         <v>0</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K41" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L41" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M41" s="14">
         <f t="shared" si="0"/>
@@ -4278,13 +4283,13 @@
         <v>80</v>
       </c>
       <c r="P41" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q41" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R41" s="76" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S41" s="77"/>
       <c r="T41" s="12"/>
@@ -4292,13 +4297,13 @@
         <v>0</v>
       </c>
       <c r="AK41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="96"/>
       <c r="C42" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="67">
         <v>1</v>
@@ -4319,10 +4324,10 @@
         <v>1</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L42" s="56" t="s">
         <v>7</v>
@@ -4339,13 +4344,13 @@
         <v>80</v>
       </c>
       <c r="P42" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q42" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R42" s="76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="S42" s="77"/>
       <c r="T42" s="12"/>
@@ -4353,15 +4358,15 @@
         <v>0</v>
       </c>
       <c r="AK42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" s="67">
         <v>1</v>
@@ -4376,19 +4381,19 @@
         <v>1</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K43" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L43" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M43" s="14">
         <f t="shared" si="0"/>
@@ -4402,31 +4407,31 @@
         <v>90</v>
       </c>
       <c r="P43" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q43" s="69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R43" s="76" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S43" s="77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T43" s="12"/>
       <c r="W43" s="14">
         <v>1</v>
       </c>
       <c r="AK43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="67">
         <v>1</v>
@@ -4441,19 +4446,19 @@
         <v>0</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K44" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L44" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M44" s="14">
         <f t="shared" si="0"/>
@@ -4464,16 +4469,16 @@
         <v>A0</v>
       </c>
       <c r="O44" s="50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P44" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q44" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R44" s="76" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="S44" s="77"/>
       <c r="T44" s="12"/>
@@ -4481,15 +4486,15 @@
         <v>0</v>
       </c>
       <c r="AK44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="93" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" s="67">
         <v>1</v>
@@ -4510,13 +4515,13 @@
         <v>0</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L45" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M45" s="14">
         <f t="shared" si="0"/>
@@ -4527,16 +4532,16 @@
         <v>B0</v>
       </c>
       <c r="O45" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P45" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q45" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R45" s="76" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="S45" s="77"/>
       <c r="T45" s="12"/>
@@ -4544,13 +4549,13 @@
         <v>0</v>
       </c>
       <c r="AK45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="93"/>
       <c r="C46" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="67">
         <v>1</v>
@@ -4571,10 +4576,10 @@
         <v>1</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L46" s="56" t="s">
         <v>7</v>
@@ -4588,16 +4593,16 @@
         <v>B4</v>
       </c>
       <c r="O46" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P46" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q46" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R46" s="76" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S46" s="77"/>
       <c r="T46" s="12"/>
@@ -4605,13 +4610,13 @@
         <v>0</v>
       </c>
       <c r="AK46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="93"/>
       <c r="C47" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D47" s="67">
         <v>1</v>
@@ -4632,13 +4637,13 @@
         <v>0</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L47" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M47" s="14">
         <f t="shared" si="0"/>
@@ -4649,16 +4654,16 @@
         <v>B8</v>
       </c>
       <c r="O47" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P47" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q47" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R47" s="76" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S47" s="77"/>
       <c r="T47" s="12"/>
@@ -4666,13 +4671,13 @@
         <v>0</v>
       </c>
       <c r="AK47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="93"/>
       <c r="C48" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" s="67">
         <v>1</v>
@@ -4693,10 +4698,10 @@
         <v>1</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K48" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L48" s="56" t="s">
         <v>7</v>
@@ -4710,16 +4715,16 @@
         <v>BC</v>
       </c>
       <c r="O48" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P48" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q48" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R48" s="76" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S48" s="77"/>
       <c r="T48" s="12"/>
@@ -4727,15 +4732,15 @@
         <v>0</v>
       </c>
       <c r="AK48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D49" s="67">
         <v>1</v>
@@ -4750,19 +4755,19 @@
         <v>0</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L49" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M49" s="14">
         <f t="shared" si="0"/>
@@ -4773,16 +4778,16 @@
         <v>C0</v>
       </c>
       <c r="O49" s="47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P49" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q49" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R49" s="76" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="S49" s="77"/>
       <c r="T49" s="12"/>
@@ -4790,15 +4795,15 @@
         <v>0</v>
       </c>
       <c r="AK49" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="67">
         <v>1</v>
@@ -4813,19 +4818,19 @@
         <v>1</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L50" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" si="0"/>
@@ -4836,16 +4841,16 @@
         <v>D0</v>
       </c>
       <c r="O50" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="P50" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="P50" s="42" t="s">
-        <v>81</v>
-      </c>
       <c r="Q50" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R50" s="76" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="S50" s="77"/>
       <c r="T50" s="12"/>
@@ -4853,15 +4858,15 @@
         <v>0</v>
       </c>
       <c r="AK50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" s="67">
         <v>1</v>
@@ -4882,13 +4887,13 @@
         <v>0</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K51" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L51" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M51" s="14">
         <f t="shared" si="0"/>
@@ -4899,16 +4904,16 @@
         <v>E0</v>
       </c>
       <c r="O51" s="49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P51" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q51" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R51" s="76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="S51" s="77"/>
       <c r="T51" s="12"/>
@@ -4916,13 +4921,13 @@
         <v>0</v>
       </c>
       <c r="AK51" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="91"/>
       <c r="C52" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" s="67">
         <v>1</v>
@@ -4943,13 +4948,13 @@
         <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L52" s="56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M52" s="14">
         <f t="shared" si="0"/>
@@ -4960,16 +4965,16 @@
         <v>E4</v>
       </c>
       <c r="O52" s="49" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P52" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q52" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R52" s="76" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S52" s="77"/>
       <c r="T52" s="12"/>
@@ -4977,15 +4982,15 @@
         <v>0</v>
       </c>
       <c r="AK52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="92" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53" s="67">
         <v>1</v>
@@ -5006,13 +5011,13 @@
         <v>0</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L53" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M53" s="14">
         <f t="shared" si="0"/>
@@ -5023,16 +5028,16 @@
         <v>E8</v>
       </c>
       <c r="O53" s="53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P53" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q53" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R53" s="76" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S53" s="77"/>
       <c r="T53" s="12"/>
@@ -5040,13 +5045,13 @@
         <v>0</v>
       </c>
       <c r="AK53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="92"/>
       <c r="C54" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="67">
         <v>1</v>
@@ -5067,10 +5072,10 @@
         <v>1</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K54" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L54" s="56" t="s">
         <v>7</v>
@@ -5084,16 +5089,16 @@
         <v>EC</v>
       </c>
       <c r="O54" s="53" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P54" s="42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q54" s="69" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R54" s="76" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="S54" s="77"/>
       <c r="T54" s="12"/>
@@ -5101,12 +5106,12 @@
         <v>0</v>
       </c>
       <c r="AK54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" s="39" t="s">
         <v>4</v>
@@ -5136,7 +5141,7 @@
         <v>0</v>
       </c>
       <c r="L55" s="57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M55" s="41">
         <f t="shared" si="0"/>
@@ -5147,20 +5152,20 @@
         <v>F0</v>
       </c>
       <c r="O55" s="51" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P55" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q55" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R55" s="78"/>
       <c r="S55" s="79"/>
       <c r="T55" s="12"/>
       <c r="W55" s="39"/>
       <c r="AK55" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add stack manipulation opcodes
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E24C9-7B51-4AC8-8E0B-AEC5ACAB92E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8351EF0E-1A9A-4FDC-96BE-F364EA1AEF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="158">
   <si>
     <t>Byte 2</t>
   </si>
@@ -135,9 +135,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>PUSH</t>
-  </si>
-  <si>
     <t>STORE</t>
   </si>
   <si>
@@ -529,6 +526,12 @@
   </si>
   <si>
     <t>LDA</t>
+  </si>
+  <si>
+    <t>PSH</t>
+  </si>
+  <si>
+    <t>PEK</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1438,6 +1441,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1824,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C23" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,10 +1871,10 @@
     </row>
     <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="31">
         <v>7</v>
@@ -1901,41 +1907,41 @@
         <v>13</v>
       </c>
       <c r="N3" s="58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R3" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="S3" s="73" t="s">
         <v>90</v>
-      </c>
-      <c r="S3" s="73" t="s">
-        <v>91</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W3" s="72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="X3" s="97" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
-        <v>20/45</v>
+        <v>23/46</v>
       </c>
       <c r="AK3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>2</v>
@@ -1979,24 +1985,24 @@
         <v>0</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q4" s="71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R4" s="74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S4" s="75"/>
       <c r="T4" s="12"/>
       <c r="U4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W4" s="62">
         <v>1</v>
       </c>
       <c r="AK4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2043,24 +2049,24 @@
         <v>0</v>
       </c>
       <c r="P5" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q5" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R5" s="76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S5" s="77"/>
       <c r="T5" s="12"/>
       <c r="U5" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W5" s="14">
         <v>1</v>
       </c>
       <c r="AK5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2107,24 +2113,24 @@
         <v>0</v>
       </c>
       <c r="P6" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q6" s="69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R6" s="76" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S6" s="77"/>
       <c r="T6" s="12"/>
       <c r="U6" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W6" s="14">
         <v>1</v>
       </c>
       <c r="AK6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2171,24 +2177,24 @@
         <v>0</v>
       </c>
       <c r="P7" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q7" s="69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R7" s="76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S7" s="77"/>
       <c r="T7" s="12"/>
       <c r="U7" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W7" s="14">
         <v>1</v>
       </c>
       <c r="AK7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2235,24 +2241,24 @@
         <v>0</v>
       </c>
       <c r="P8" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q8" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R8" s="76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S8" s="77"/>
       <c r="T8" s="12"/>
       <c r="U8" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W8" s="14">
         <v>1</v>
       </c>
       <c r="AK8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2299,24 +2305,24 @@
         <v>0</v>
       </c>
       <c r="P9" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q9" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R9" s="76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S9" s="77"/>
       <c r="T9" s="12"/>
       <c r="U9" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W9" s="14">
         <v>1</v>
       </c>
       <c r="AK9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2363,20 +2369,20 @@
         <v>0</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R10" s="76"/>
       <c r="S10" s="77"/>
       <c r="T10" s="12"/>
       <c r="U10" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W10" s="15"/>
       <c r="AK10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2423,25 +2429,25 @@
         <v>0</v>
       </c>
       <c r="P11" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q11" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R11" s="76"/>
       <c r="S11" s="77"/>
       <c r="T11" s="12"/>
       <c r="U11" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W11" s="15"/>
       <c r="AK11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>8</v>
@@ -2485,16 +2491,16 @@
         <v>8</v>
       </c>
       <c r="P12" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q12" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R12" s="76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S12" s="77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T12" s="12"/>
       <c r="U12" s="64"/>
@@ -2502,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="AK12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2549,17 +2555,17 @@
         <v>8</v>
       </c>
       <c r="P13" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q13" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R13" s="76"/>
       <c r="S13" s="77"/>
       <c r="T13" s="12"/>
       <c r="W13" s="15"/>
       <c r="AK13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2606,13 +2612,13 @@
         <v>8</v>
       </c>
       <c r="P14" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q14" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R14" s="76" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S14" s="77"/>
       <c r="T14" s="12"/>
@@ -2620,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="AK14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2667,13 +2673,13 @@
         <v>8</v>
       </c>
       <c r="P15" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q15" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R15" s="76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S15" s="77"/>
       <c r="T15" s="12"/>
@@ -2681,7 +2687,7 @@
         <v>1</v>
       </c>
       <c r="AK15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2728,13 +2734,13 @@
         <v>8</v>
       </c>
       <c r="P16" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q16" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R16" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S16" s="77"/>
       <c r="T16" s="12"/>
@@ -2742,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="AK16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2789,13 +2795,13 @@
         <v>8</v>
       </c>
       <c r="P17" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q17" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R17" s="76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S17" s="77"/>
       <c r="T17" s="12"/>
@@ -2803,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="AK17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2850,23 +2856,23 @@
         <v>8</v>
       </c>
       <c r="P18" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q18" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R18" s="76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S18" s="77" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T18" s="12"/>
       <c r="W18" s="14">
         <v>1</v>
       </c>
       <c r="AK18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2913,23 +2919,23 @@
         <v>8</v>
       </c>
       <c r="P19" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q19" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R19" s="76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S19" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T19" s="12"/>
       <c r="W19" s="14">
         <v>1</v>
       </c>
       <c r="AK19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2978,13 +2984,13 @@
         <v>10</v>
       </c>
       <c r="P20" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q20" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R20" s="76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S20" s="77"/>
       <c r="T20" s="12"/>
@@ -2992,13 +2998,13 @@
         <v>1</v>
       </c>
       <c r="AK20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="81"/>
       <c r="C21" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="66">
         <v>0</v>
@@ -3039,13 +3045,13 @@
         <v>10</v>
       </c>
       <c r="P21" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q21" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R21" s="76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S21" s="77"/>
       <c r="T21" s="12"/>
@@ -3053,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="AK21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3100,27 +3106,27 @@
         <v>10</v>
       </c>
       <c r="P22" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q22" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R22" s="76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S22" s="77"/>
       <c r="T22" s="12"/>
       <c r="W22" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="81"/>
-      <c r="C23" s="15" t="s">
-        <v>4</v>
+      <c r="C23" s="98" t="s">
+        <v>157</v>
       </c>
       <c r="D23" s="66">
         <v>0</v>
@@ -3140,11 +3146,11 @@
       <c r="I23" s="3">
         <v>1</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K23" s="17" t="s">
-        <v>4</v>
+      <c r="J23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="L23" s="56" t="s">
         <v>24</v>
@@ -3161,22 +3167,24 @@
         <v>10</v>
       </c>
       <c r="P23" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q23" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R23" s="76"/>
       <c r="S23" s="77"/>
       <c r="T23" s="12"/>
-      <c r="W23" s="15"/>
+      <c r="W23" s="15">
+        <v>1</v>
+      </c>
       <c r="AK23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>4</v>
@@ -3220,23 +3228,23 @@
         <v>20</v>
       </c>
       <c r="P24" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q24" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R24" s="76"/>
       <c r="S24" s="77"/>
       <c r="T24" s="12"/>
       <c r="W24" s="15"/>
       <c r="AK24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="80"/>
       <c r="C25" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="66">
         <v>0</v>
@@ -3277,13 +3285,13 @@
         <v>20</v>
       </c>
       <c r="P25" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q25" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R25" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S25" s="77"/>
       <c r="T25" s="12"/>
@@ -3291,13 +3299,13 @@
         <v>1</v>
       </c>
       <c r="AK25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="80"/>
       <c r="C26" s="14" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
       <c r="D26" s="66">
         <v>0</v>
@@ -3338,21 +3346,21 @@
         <v>20</v>
       </c>
       <c r="P26" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q26" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R26" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S26" s="77"/>
       <c r="T26" s="12"/>
       <c r="W26" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3399,25 +3407,25 @@
         <v>20</v>
       </c>
       <c r="P27" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q27" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R27" s="76"/>
       <c r="S27" s="77"/>
       <c r="T27" s="12"/>
       <c r="W27" s="15"/>
       <c r="AK27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="66">
         <v>0</v>
@@ -3458,13 +3466,13 @@
         <v>30</v>
       </c>
       <c r="P28" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q28" s="69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R28" s="76" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S28" s="77"/>
       <c r="T28" s="12"/>
@@ -3472,15 +3480,15 @@
         <v>1</v>
       </c>
       <c r="AK28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="66">
         <v>0</v>
@@ -3521,29 +3529,29 @@
         <v>40</v>
       </c>
       <c r="P29" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q29" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R29" s="76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S29" s="77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T29" s="12"/>
       <c r="W29" s="14">
         <v>1</v>
       </c>
       <c r="AK29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="93"/>
       <c r="C30" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="67">
         <v>0</v>
@@ -3584,29 +3592,29 @@
         <v>40</v>
       </c>
       <c r="P30" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q30" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R30" s="76" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S30" s="77" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T30" s="12"/>
       <c r="W30" s="14">
         <v>0</v>
       </c>
       <c r="AK30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="93"/>
       <c r="C31" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="67">
         <v>0</v>
@@ -3647,29 +3655,29 @@
         <v>40</v>
       </c>
       <c r="P31" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q31" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R31" s="76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S31" s="77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T31" s="12"/>
       <c r="W31" s="14">
         <v>1</v>
       </c>
       <c r="AK31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="93"/>
       <c r="C32" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="67">
         <v>0</v>
@@ -3710,31 +3718,31 @@
         <v>40</v>
       </c>
       <c r="P32" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q32" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R32" s="76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S32" s="77" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T32" s="12"/>
       <c r="W32" s="14">
         <v>0</v>
       </c>
       <c r="AK32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="94" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="67">
         <v>0</v>
@@ -3775,29 +3783,29 @@
         <v>50</v>
       </c>
       <c r="P33" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q33" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R33" s="76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S33" s="77" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T33" s="12"/>
       <c r="W33" s="14">
         <v>0</v>
       </c>
       <c r="AK33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="94"/>
       <c r="C34" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="67">
         <v>0</v>
@@ -3838,31 +3846,31 @@
         <v>60</v>
       </c>
       <c r="P34" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q34" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R34" s="76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S34" s="77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T34" s="12"/>
       <c r="W34" s="14">
         <v>0</v>
       </c>
       <c r="AK34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="95" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="67">
         <v>0</v>
@@ -3903,29 +3911,29 @@
         <v>70</v>
       </c>
       <c r="P35" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q35" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R35" s="76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S35" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T35" s="12"/>
       <c r="W35" s="14">
         <v>0</v>
       </c>
       <c r="AK35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="95"/>
       <c r="C36" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D36" s="67">
         <v>0</v>
@@ -3966,29 +3974,29 @@
         <v>70</v>
       </c>
       <c r="P36" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q36" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R36" s="76" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S36" s="77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T36" s="12"/>
       <c r="W36" s="14">
         <v>0</v>
       </c>
       <c r="AK36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="95"/>
       <c r="C37" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="67">
         <v>0</v>
@@ -4029,29 +4037,29 @@
         <v>70</v>
       </c>
       <c r="P37" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q37" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R37" s="76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S37" s="77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T37" s="12"/>
       <c r="W37" s="14">
         <v>0</v>
       </c>
       <c r="AK37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="95"/>
       <c r="C38" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" s="67">
         <v>0</v>
@@ -4092,31 +4100,31 @@
         <v>70</v>
       </c>
       <c r="P38" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q38" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R38" s="76" t="s">
+        <v>140</v>
+      </c>
+      <c r="S38" s="77" t="s">
         <v>141</v>
-      </c>
-      <c r="S38" s="77" t="s">
-        <v>142</v>
       </c>
       <c r="T38" s="12"/>
       <c r="W38" s="14">
         <v>0</v>
       </c>
       <c r="AK38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="96" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D39" s="67">
         <v>1</v>
@@ -4157,29 +4165,29 @@
         <v>80</v>
       </c>
       <c r="P39" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q39" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R39" s="76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S39" s="77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T39" s="12"/>
       <c r="W39" s="14">
         <v>0</v>
       </c>
       <c r="AK39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="96"/>
       <c r="C40" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="67">
         <v>1</v>
@@ -4220,29 +4228,29 @@
         <v>80</v>
       </c>
       <c r="P40" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q40" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R40" s="76" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S40" s="77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T40" s="12"/>
       <c r="W40" s="14">
         <v>0</v>
       </c>
       <c r="AK40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="96"/>
       <c r="C41" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="67">
         <v>1</v>
@@ -4283,13 +4291,13 @@
         <v>80</v>
       </c>
       <c r="P41" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q41" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R41" s="76" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S41" s="77"/>
       <c r="T41" s="12"/>
@@ -4297,13 +4305,13 @@
         <v>0</v>
       </c>
       <c r="AK41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="96"/>
       <c r="C42" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" s="67">
         <v>1</v>
@@ -4344,13 +4352,13 @@
         <v>80</v>
       </c>
       <c r="P42" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q42" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R42" s="76" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S42" s="77"/>
       <c r="T42" s="12"/>
@@ -4358,15 +4366,15 @@
         <v>0</v>
       </c>
       <c r="AK42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="67">
         <v>1</v>
@@ -4407,31 +4415,31 @@
         <v>90</v>
       </c>
       <c r="P43" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q43" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R43" s="76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S43" s="77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T43" s="12"/>
       <c r="W43" s="14">
         <v>1</v>
       </c>
       <c r="AK43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="67">
         <v>1</v>
@@ -4469,16 +4477,16 @@
         <v>A0</v>
       </c>
       <c r="O44" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P44" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q44" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R44" s="76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S44" s="77"/>
       <c r="T44" s="12"/>
@@ -4486,15 +4494,15 @@
         <v>0</v>
       </c>
       <c r="AK44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="67">
         <v>1</v>
@@ -4532,16 +4540,16 @@
         <v>B0</v>
       </c>
       <c r="O45" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P45" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q45" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R45" s="76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S45" s="77"/>
       <c r="T45" s="12"/>
@@ -4549,13 +4557,13 @@
         <v>0</v>
       </c>
       <c r="AK45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="93"/>
       <c r="C46" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="67">
         <v>1</v>
@@ -4593,16 +4601,16 @@
         <v>B4</v>
       </c>
       <c r="O46" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P46" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q46" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R46" s="76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S46" s="77"/>
       <c r="T46" s="12"/>
@@ -4610,13 +4618,13 @@
         <v>0</v>
       </c>
       <c r="AK46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="93"/>
       <c r="C47" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="67">
         <v>1</v>
@@ -4654,16 +4662,16 @@
         <v>B8</v>
       </c>
       <c r="O47" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P47" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q47" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R47" s="76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S47" s="77"/>
       <c r="T47" s="12"/>
@@ -4671,13 +4679,13 @@
         <v>0</v>
       </c>
       <c r="AK47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="93"/>
       <c r="C48" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="67">
         <v>1</v>
@@ -4715,16 +4723,16 @@
         <v>BC</v>
       </c>
       <c r="O48" s="45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P48" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q48" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R48" s="76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S48" s="77"/>
       <c r="T48" s="12"/>
@@ -4732,15 +4740,15 @@
         <v>0</v>
       </c>
       <c r="AK48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D49" s="67">
         <v>1</v>
@@ -4778,16 +4786,16 @@
         <v>C0</v>
       </c>
       <c r="O49" s="47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P49" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q49" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R49" s="76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S49" s="77"/>
       <c r="T49" s="12"/>
@@ -4795,15 +4803,15 @@
         <v>0</v>
       </c>
       <c r="AK49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="67">
         <v>1</v>
@@ -4841,16 +4849,16 @@
         <v>D0</v>
       </c>
       <c r="O50" s="48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P50" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q50" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R50" s="76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S50" s="77"/>
       <c r="T50" s="12"/>
@@ -4858,15 +4866,15 @@
         <v>0</v>
       </c>
       <c r="AK50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D51" s="67">
         <v>1</v>
@@ -4904,16 +4912,16 @@
         <v>E0</v>
       </c>
       <c r="O51" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P51" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q51" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R51" s="76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S51" s="77"/>
       <c r="T51" s="12"/>
@@ -4921,13 +4929,13 @@
         <v>0</v>
       </c>
       <c r="AK51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="91"/>
       <c r="C52" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" s="67">
         <v>1</v>
@@ -4965,16 +4973,16 @@
         <v>E4</v>
       </c>
       <c r="O52" s="49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P52" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q52" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R52" s="76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S52" s="77"/>
       <c r="T52" s="12"/>
@@ -4982,15 +4990,15 @@
         <v>0</v>
       </c>
       <c r="AK52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" s="67">
         <v>1</v>
@@ -5028,16 +5036,16 @@
         <v>E8</v>
       </c>
       <c r="O53" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P53" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q53" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R53" s="76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S53" s="77"/>
       <c r="T53" s="12"/>
@@ -5045,13 +5053,13 @@
         <v>0</v>
       </c>
       <c r="AK53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="92"/>
       <c r="C54" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D54" s="67">
         <v>1</v>
@@ -5089,16 +5097,16 @@
         <v>EC</v>
       </c>
       <c r="O54" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P54" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q54" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R54" s="76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S54" s="77"/>
       <c r="T54" s="12"/>
@@ -5106,12 +5114,12 @@
         <v>0</v>
       </c>
       <c r="AK54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="39" t="s">
         <v>4</v>
@@ -5152,20 +5160,20 @@
         <v>F0</v>
       </c>
       <c r="O55" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P55" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q55" s="70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R55" s="78"/>
       <c r="S55" s="79"/>
       <c r="T55" s="12"/>
       <c r="W55" s="39"/>
       <c r="AK55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plan for introduction of indirect addressing
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B869A67E-6805-4C63-ADEF-567F72C70509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734396A-76A0-4832-AEFD-68DADA09EC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13944" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="167">
   <si>
     <t>Byte 2</t>
   </si>
@@ -535,6 +535,30 @@
   </si>
   <si>
     <t>Analysis</t>
+  </si>
+  <si>
+    <t>Peek top stack value into register</t>
+  </si>
+  <si>
+    <t>INDIRECT</t>
+  </si>
+  <si>
+    <t>LDX</t>
+  </si>
+  <si>
+    <t>STX</t>
+  </si>
+  <si>
+    <t>reg + imm</t>
+  </si>
+  <si>
+    <t>Load value pointed to by address in (reg + imm) into rd</t>
+  </si>
+  <si>
+    <t>Store value in rs into memory at address into (reg + imm)</t>
+  </si>
+  <si>
+    <t>The low 2 bits are used for the register idx, the remaining high 6 bits are for the immediate offset (max 63)</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1395,6 +1419,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1404,9 +1446,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,23 +1467,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1832,48 +1859,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="Z55" sqref="Z55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K12" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" customWidth="1"/>
-    <col min="4" max="11" width="3.81640625" customWidth="1"/>
-    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="11" width="3.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="7.1796875" customWidth="1"/>
-    <col min="15" max="15" width="5.81640625" customWidth="1"/>
-    <col min="16" max="16" width="5.453125" customWidth="1"/>
-    <col min="17" max="17" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="87.08984375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="1" customWidth="1"/>
-    <col min="21" max="21" width="17.36328125" customWidth="1"/>
-    <col min="22" max="22" width="0.90625" customWidth="1"/>
-    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.90625" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="87.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" customWidth="1"/>
+    <col min="22" max="22" width="0.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.88671875" customWidth="1"/>
     <col min="25" max="25" width="1" customWidth="1"/>
-    <col min="31" max="31" width="14.54296875" customWidth="1"/>
-    <col min="32" max="32" width="44.1796875" customWidth="1"/>
+    <col min="31" max="31" width="14.5546875" customWidth="1"/>
+    <col min="32" max="32" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="83"/>
+    <row r="1" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="89"/>
     </row>
-    <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>68</v>
       </c>
@@ -1937,21 +1964,21 @@
       </c>
       <c r="X3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
-        <v>46/46</v>
+        <v>46/48</v>
       </c>
       <c r="Z3" s="72" t="s">
         <v>158</v>
       </c>
       <c r="AA3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(Z4:Z55,1),"0"), TEXT(COUNTIF(Z4:Z55,"&gt;=0"),"0"))</f>
-        <v>46/46</v>
+        <v>46/48</v>
       </c>
       <c r="AK3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="86" t="s">
+    <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="91" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -2019,8 +2046,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="87"/>
+    <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="92"/>
       <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
@@ -2086,8 +2113,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="87"/>
+    <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="92"/>
       <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
@@ -2153,8 +2180,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="87"/>
+    <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="92"/>
       <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
@@ -2220,8 +2247,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="87"/>
+    <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="92"/>
       <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
@@ -2287,8 +2314,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="87"/>
+    <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="92"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
@@ -2354,8 +2381,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="87"/>
+    <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="92"/>
       <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
@@ -2415,8 +2442,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="88"/>
+    <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="93"/>
       <c r="C11" s="15" t="s">
         <v>4</v>
       </c>
@@ -2476,8 +2503,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="89" t="s">
+    <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="94" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2545,8 +2572,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="90"/>
+    <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="95"/>
       <c r="C13" s="15" t="s">
         <v>4</v>
       </c>
@@ -2603,8 +2630,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="90"/>
+    <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="95"/>
       <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
@@ -2667,8 +2694,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="90"/>
+    <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="95"/>
       <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
@@ -2731,8 +2758,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="90"/>
+    <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="95"/>
       <c r="C16" s="14" t="s">
         <v>10</v>
       </c>
@@ -2795,8 +2822,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="90"/>
+    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="95"/>
       <c r="C17" s="14" t="s">
         <v>9</v>
       </c>
@@ -2859,8 +2886,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="90"/>
+    <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="95"/>
       <c r="C18" s="14" t="s">
         <v>6</v>
       </c>
@@ -2925,8 +2952,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="91"/>
+    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="96"/>
       <c r="C19" s="14" t="s">
         <v>5</v>
       </c>
@@ -2991,8 +3018,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="85" t="s">
+    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="90" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -3057,8 +3084,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="85"/>
+    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="90"/>
       <c r="C21" s="14" t="s">
         <v>155</v>
       </c>
@@ -3121,8 +3148,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="85"/>
+    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="90"/>
       <c r="C22" s="14" t="s">
         <v>21</v>
       </c>
@@ -3185,8 +3212,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="85"/>
+    <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="90"/>
       <c r="C23" s="14" t="s">
         <v>157</v>
       </c>
@@ -3234,7 +3261,9 @@
       <c r="Q23" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R23" s="76"/>
+      <c r="R23" s="76" t="s">
+        <v>159</v>
+      </c>
       <c r="S23" s="77"/>
       <c r="T23" s="12"/>
       <c r="W23" s="15">
@@ -3247,12 +3276,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="84" t="s">
+    <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>4</v>
+      <c r="C24" s="14" t="s">
+        <v>156</v>
       </c>
       <c r="D24" s="66">
         <v>0</v>
@@ -3272,17 +3301,17 @@
       <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>4</v>
+      <c r="J24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="L24" s="56" t="s">
         <v>24</v>
       </c>
       <c r="M24" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M24" si="1">IF(L24="NA",1,2)</f>
         <v>1</v>
       </c>
       <c r="N24" s="60" t="str" cm="1">
@@ -3298,17 +3327,23 @@
       <c r="Q24" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R24" s="76"/>
+      <c r="R24" s="76" t="s">
+        <v>110</v>
+      </c>
       <c r="S24" s="77"/>
       <c r="T24" s="12"/>
-      <c r="W24" s="15"/>
-      <c r="Z24" s="15"/>
+      <c r="W24" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="14">
+        <v>1</v>
+      </c>
       <c r="AK24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="84"/>
+    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="98"/>
       <c r="C25" s="14" t="s">
         <v>154</v>
       </c>
@@ -3371,10 +3406,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="84"/>
+    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="82" t="s">
+        <v>160</v>
+      </c>
       <c r="C26" s="14" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D26" s="66">
         <v>0</v>
@@ -3394,24 +3431,24 @@
       <c r="I26" s="3">
         <v>0</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="21" t="s">
-        <v>20</v>
+      <c r="J26" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="L26" s="56" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="M26" s="14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N26" s="60" t="str" cm="1">
         <f t="array" ref="N26">DEC2HEX(SUMPRODUCT(D26:K26,2^($D$3:$K$3)),2)</f>
         <v>28</v>
       </c>
-      <c r="O26" s="49">
+      <c r="O26" s="53">
         <v>20</v>
       </c>
       <c r="P26" s="42" t="s">
@@ -3421,24 +3458,26 @@
         <v>88</v>
       </c>
       <c r="R26" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="S26" s="77"/>
+        <v>164</v>
+      </c>
+      <c r="S26" s="77" t="s">
+        <v>166</v>
+      </c>
       <c r="T26" s="12"/>
       <c r="W26" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="84"/>
-      <c r="C27" s="15" t="s">
-        <v>4</v>
+    <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="82"/>
+      <c r="C27" s="14" t="s">
+        <v>162</v>
       </c>
       <c r="D27" s="66">
         <v>0</v>
@@ -3458,24 +3497,24 @@
       <c r="I27" s="3">
         <v>1</v>
       </c>
-      <c r="J27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K27" s="17" t="s">
-        <v>4</v>
+      <c r="J27" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="21" t="s">
+        <v>20</v>
       </c>
       <c r="L27" s="56" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="M27" s="14">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N27" s="60" t="str" cm="1">
         <f t="array" ref="N27">DEC2HEX(SUMPRODUCT(D27:K27,2^($D$3:$K$3)),2)</f>
         <v>2C</v>
       </c>
-      <c r="O27" s="49">
+      <c r="O27" s="53">
         <v>20</v>
       </c>
       <c r="P27" s="42" t="s">
@@ -3484,16 +3523,24 @@
       <c r="Q27" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R27" s="76"/>
-      <c r="S27" s="77"/>
+      <c r="R27" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="S27" s="77" t="s">
+        <v>166</v>
+      </c>
       <c r="T27" s="12"/>
-      <c r="W27" s="15"/>
-      <c r="Z27" s="15"/>
+      <c r="W27" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="15">
+        <v>0</v>
+      </c>
       <c r="AK27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="36" t="s">
         <v>51</v>
       </c>
@@ -3559,8 +3606,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="94" t="s">
+    <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="83" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -3627,8 +3674,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="94"/>
+    <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="83"/>
       <c r="C30" s="14" t="s">
         <v>35</v>
       </c>
@@ -3693,8 +3740,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="94"/>
+    <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="83"/>
       <c r="C31" s="14" t="s">
         <v>36</v>
       </c>
@@ -3759,8 +3806,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="94"/>
+    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="83"/>
       <c r="C32" s="14" t="s">
         <v>37</v>
       </c>
@@ -3825,8 +3872,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="95" t="s">
+    <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="84" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -3893,8 +3940,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="95"/>
+    <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="84"/>
       <c r="C34" s="14" t="s">
         <v>32</v>
       </c>
@@ -3959,8 +4006,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="96" t="s">
+    <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="85" t="s">
         <v>62</v>
       </c>
       <c r="C35" s="14" t="s">
@@ -4027,8 +4074,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="96"/>
+    <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="85"/>
       <c r="C36" s="14" t="s">
         <v>30</v>
       </c>
@@ -4093,8 +4140,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="96"/>
+    <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="85"/>
       <c r="C37" s="14" t="s">
         <v>60</v>
       </c>
@@ -4159,8 +4206,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="96"/>
+    <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="85"/>
       <c r="C38" s="14" t="s">
         <v>61</v>
       </c>
@@ -4225,8 +4272,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="97" t="s">
+    <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="86" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -4293,8 +4340,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="97"/>
+    <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="86"/>
       <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
@@ -4359,8 +4406,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="97"/>
+    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="86"/>
       <c r="C41" s="14" t="s">
         <v>42</v>
       </c>
@@ -4423,8 +4470,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="97"/>
+    <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="86"/>
       <c r="C42" s="14" t="s">
         <v>43</v>
       </c>
@@ -4487,7 +4534,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="35" t="s">
         <v>52</v>
       </c>
@@ -4555,7 +4602,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="36" t="s">
         <v>27</v>
       </c>
@@ -4621,8 +4668,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="94" t="s">
+    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="83" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="14" t="s">
@@ -4687,8 +4734,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="94"/>
+    <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="83"/>
       <c r="C46" s="14" t="s">
         <v>45</v>
       </c>
@@ -4751,8 +4798,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="94"/>
+    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="83"/>
       <c r="C47" s="14" t="s">
         <v>46</v>
       </c>
@@ -4815,8 +4862,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="94"/>
+    <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="83"/>
       <c r="C48" s="14" t="s">
         <v>47</v>
       </c>
@@ -4879,7 +4926,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="37" t="s">
         <v>28</v>
       </c>
@@ -4945,7 +4992,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="34" t="s">
         <v>48</v>
       </c>
@@ -5011,8 +5058,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="92" t="s">
+    <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="81" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -5077,8 +5124,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="92"/>
+    <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="81"/>
       <c r="C52" s="14" t="s">
         <v>39</v>
       </c>
@@ -5141,8 +5188,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="93" t="s">
+    <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="82" t="s">
         <v>59</v>
       </c>
       <c r="C53" s="14" t="s">
@@ -5207,8 +5254,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="93"/>
+    <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="82"/>
       <c r="C54" s="14" t="s">
         <v>64</v>
       </c>
@@ -5271,7 +5318,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="38" t="s">
         <v>69</v>
       </c>
@@ -5332,7 +5379,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B29:B32"/>
@@ -5340,25 +5393,20 @@
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B19"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L55">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="addr">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="addr">
       <formula>NOT(ISERROR(SEARCH("addr",L4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="imm">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="imm">
       <formula>NOT(ISERROR(SEARCH("imm",L4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M55">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="2"/>
@@ -5368,18 +5416,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P55">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="FF">
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="FF">
       <formula>NOT(ISERROR(SEARCH("FF",P4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="FC">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="FC">
       <formula>NOT(ISERROR(SEARCH("FC",P4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="F0">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="F0">
       <formula>NOT(ISERROR(SEARCH("F0",P4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:W55">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5388,7 +5436,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z4:Z55">
+  <conditionalFormatting sqref="Z4:Z23 Z25:Z55">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF5050"/>
+        <color theme="9" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fix org directive issue
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734396A-76A0-4832-AEFD-68DADA09EC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF2C160-A924-46E7-90E0-951236982CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
@@ -558,7 +558,7 @@
     <t>Store value in rs into memory at address into (reg + imm)</t>
   </si>
   <si>
-    <t>The low 2 bits are used for the register idx, the remaining high 6 bits are for the immediate offset (max 63)</t>
+    <t>The low 2 bits are used for the register idx, the remaining high 6 bits are for the immediate offset (max 63, only positive)</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K12" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="AD36" sqref="AD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1875,8 +1875,8 @@
     <col min="15" max="15" width="5.77734375" customWidth="1"/>
     <col min="16" max="16" width="5.44140625" customWidth="1"/>
     <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="47" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="87.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="87.109375" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="6.6640625" customWidth="1"/>
     <col min="21" max="21" width="17.33203125" customWidth="1"/>
     <col min="22" max="22" width="0.88671875" customWidth="1"/>
@@ -1964,14 +1964,14 @@
       </c>
       <c r="X3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
-        <v>46/48</v>
+        <v>48/48</v>
       </c>
       <c r="Z3" s="72" t="s">
         <v>158</v>
       </c>
       <c r="AA3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(Z4:Z55,1),"0"), TEXT(COUNTIF(Z4:Z55,"&gt;=0"),"0"))</f>
-        <v>46/48</v>
+        <v>48/48</v>
       </c>
       <c r="AK3" t="s">
         <v>88</v>
@@ -3465,10 +3465,10 @@
       </c>
       <c r="T26" s="12"/>
       <c r="W26" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK26" t="s">
         <v>88</v>
@@ -3531,10 +3531,10 @@
       </c>
       <c r="T27" s="12"/>
       <c r="W27" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z27" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK27" t="s">
         <v>88</v>

</xml_diff>

<commit_message>
Update ISA to include interrupts
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF2C160-A924-46E7-90E0-951236982CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2B7DF9-728E-4E4E-AE72-B317323B6C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="173">
   <si>
     <t>Byte 2</t>
   </si>
@@ -559,6 +559,24 @@
   </si>
   <si>
     <t>The low 2 bits are used for the register idx, the remaining high 6 bits are for the immediate offset (max 63, only positive)</t>
+  </si>
+  <si>
+    <t>SEI</t>
+  </si>
+  <si>
+    <t>CLI</t>
+  </si>
+  <si>
+    <t>RTI</t>
+  </si>
+  <si>
+    <t>Set interrupt disable</t>
+  </si>
+  <si>
+    <t>Clear interrup disable</t>
+  </si>
+  <si>
+    <t>Return from interrupt</t>
   </si>
 </sst>
 </file>
@@ -1419,12 +1437,48 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1436,42 +1490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1859,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="AD36" sqref="AD36"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1874,9 +1892,9 @@
     <col min="14" max="14" width="7.21875" customWidth="1"/>
     <col min="15" max="15" width="5.77734375" customWidth="1"/>
     <col min="16" max="16" width="5.44140625" customWidth="1"/>
-    <col min="17" max="17" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="47" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="87.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.21875" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" customWidth="1"/>
     <col min="20" max="20" width="6.6640625" customWidth="1"/>
     <col min="21" max="21" width="17.33203125" customWidth="1"/>
     <col min="22" max="22" width="0.88671875" customWidth="1"/>
@@ -1889,16 +1907,16 @@
   <sheetData>
     <row r="1" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="89"/>
+      <c r="D2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="83"/>
     </row>
     <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
@@ -1964,21 +1982,21 @@
       </c>
       <c r="X3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
-        <v>48/48</v>
+        <v>48/51</v>
       </c>
       <c r="Z3" s="72" t="s">
         <v>158</v>
       </c>
       <c r="AA3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(Z4:Z55,1),"0"), TEXT(COUNTIF(Z4:Z55,"&gt;=0"),"0"))</f>
-        <v>48/48</v>
+        <v>48/51</v>
       </c>
       <c r="AK3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="85" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -2047,7 +2065,7 @@
       </c>
     </row>
     <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="92"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
@@ -2114,7 +2132,7 @@
       </c>
     </row>
     <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="92"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
@@ -2181,7 +2199,7 @@
       </c>
     </row>
     <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="92"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
@@ -2248,7 +2266,7 @@
       </c>
     </row>
     <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="92"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
@@ -2315,7 +2333,7 @@
       </c>
     </row>
     <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="92"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
@@ -2382,9 +2400,9 @@
       </c>
     </row>
     <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="92"/>
-      <c r="C10" s="15" t="s">
-        <v>4</v>
+      <c r="B10" s="86"/>
+      <c r="C10" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="D10" s="66">
         <v>0</v>
@@ -2430,22 +2448,28 @@
       <c r="Q10" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R10" s="76"/>
+      <c r="R10" s="76" t="s">
+        <v>170</v>
+      </c>
       <c r="S10" s="77"/>
       <c r="T10" s="12"/>
       <c r="U10" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="W10" s="15"/>
-      <c r="Z10" s="15"/>
+      <c r="W10" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="15">
+        <v>0</v>
+      </c>
       <c r="AK10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="93"/>
-      <c r="C11" s="15" t="s">
-        <v>4</v>
+      <c r="B11" s="87"/>
+      <c r="C11" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="D11" s="66">
         <v>0</v>
@@ -2491,20 +2515,26 @@
       <c r="Q11" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R11" s="76"/>
+      <c r="R11" s="76" t="s">
+        <v>171</v>
+      </c>
       <c r="S11" s="77"/>
       <c r="T11" s="12"/>
       <c r="U11" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="W11" s="15"/>
-      <c r="Z11" s="15"/>
+      <c r="W11" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="15">
+        <v>0</v>
+      </c>
       <c r="AK11" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="88" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2573,9 +2603,9 @@
       </c>
     </row>
     <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="95"/>
-      <c r="C13" s="15" t="s">
-        <v>4</v>
+      <c r="B13" s="89"/>
+      <c r="C13" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="D13" s="66">
         <v>0</v>
@@ -2621,17 +2651,23 @@
       <c r="Q13" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="R13" s="76"/>
+      <c r="R13" s="76" t="s">
+        <v>172</v>
+      </c>
       <c r="S13" s="77"/>
       <c r="T13" s="12"/>
-      <c r="W13" s="15"/>
-      <c r="Z13" s="15"/>
+      <c r="W13" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="15">
+        <v>0</v>
+      </c>
       <c r="AK13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="95"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
@@ -2695,7 +2731,7 @@
       </c>
     </row>
     <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="95"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
@@ -2759,7 +2795,7 @@
       </c>
     </row>
     <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="95"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="14" t="s">
         <v>10</v>
       </c>
@@ -2823,7 +2859,7 @@
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="95"/>
+      <c r="B17" s="89"/>
       <c r="C17" s="14" t="s">
         <v>9</v>
       </c>
@@ -2887,7 +2923,7 @@
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="95"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="14" t="s">
         <v>6</v>
       </c>
@@ -2953,7 +2989,7 @@
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="96"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="14" t="s">
         <v>5</v>
       </c>
@@ -3019,7 +3055,7 @@
       </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="84" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -3085,7 +3121,7 @@
       </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="90"/>
+      <c r="B21" s="84"/>
       <c r="C21" s="14" t="s">
         <v>155</v>
       </c>
@@ -3149,7 +3185,7 @@
       </c>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="90"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="14" t="s">
         <v>21</v>
       </c>
@@ -3213,7 +3249,7 @@
       </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="90"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="14" t="s">
         <v>157</v>
       </c>
@@ -3277,7 +3313,7 @@
       </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="91" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -3343,7 +3379,7 @@
       </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="98"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="14" t="s">
         <v>154</v>
       </c>
@@ -3407,7 +3443,7 @@
       </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="93" t="s">
         <v>160</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -3475,7 +3511,7 @@
       </c>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="82"/>
+      <c r="B27" s="93"/>
       <c r="C27" s="14" t="s">
         <v>162</v>
       </c>
@@ -3607,7 +3643,7 @@
       </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="95" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -3675,7 +3711,7 @@
       </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="83"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="14" t="s">
         <v>35</v>
       </c>
@@ -3741,7 +3777,7 @@
       </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="83"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="14" t="s">
         <v>36</v>
       </c>
@@ -3807,7 +3843,7 @@
       </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="83"/>
+      <c r="B32" s="95"/>
       <c r="C32" s="14" t="s">
         <v>37</v>
       </c>
@@ -3873,7 +3909,7 @@
       </c>
     </row>
     <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="96" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -3941,7 +3977,7 @@
       </c>
     </row>
     <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="84"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="14" t="s">
         <v>32</v>
       </c>
@@ -4007,7 +4043,7 @@
       </c>
     </row>
     <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="85" t="s">
+      <c r="B35" s="97" t="s">
         <v>62</v>
       </c>
       <c r="C35" s="14" t="s">
@@ -4075,7 +4111,7 @@
       </c>
     </row>
     <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="85"/>
+      <c r="B36" s="97"/>
       <c r="C36" s="14" t="s">
         <v>30</v>
       </c>
@@ -4141,7 +4177,7 @@
       </c>
     </row>
     <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="85"/>
+      <c r="B37" s="97"/>
       <c r="C37" s="14" t="s">
         <v>60</v>
       </c>
@@ -4207,7 +4243,7 @@
       </c>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="85"/>
+      <c r="B38" s="97"/>
       <c r="C38" s="14" t="s">
         <v>61</v>
       </c>
@@ -4273,7 +4309,7 @@
       </c>
     </row>
     <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="98" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -4341,7 +4377,7 @@
       </c>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="86"/>
+      <c r="B40" s="98"/>
       <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
@@ -4407,7 +4443,7 @@
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="86"/>
+      <c r="B41" s="98"/>
       <c r="C41" s="14" t="s">
         <v>42</v>
       </c>
@@ -4471,7 +4507,7 @@
       </c>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="86"/>
+      <c r="B42" s="98"/>
       <c r="C42" s="14" t="s">
         <v>43</v>
       </c>
@@ -4669,7 +4705,7 @@
       </c>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="95" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="14" t="s">
@@ -4735,7 +4771,7 @@
       </c>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="83"/>
+      <c r="B46" s="95"/>
       <c r="C46" s="14" t="s">
         <v>45</v>
       </c>
@@ -4799,7 +4835,7 @@
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="83"/>
+      <c r="B47" s="95"/>
       <c r="C47" s="14" t="s">
         <v>46</v>
       </c>
@@ -4863,7 +4899,7 @@
       </c>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="83"/>
+      <c r="B48" s="95"/>
       <c r="C48" s="14" t="s">
         <v>47</v>
       </c>
@@ -5059,7 +5095,7 @@
       </c>
     </row>
     <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="81" t="s">
+      <c r="B51" s="94" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -5125,7 +5161,7 @@
       </c>
     </row>
     <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="81"/>
+      <c r="B52" s="94"/>
       <c r="C52" s="14" t="s">
         <v>39</v>
       </c>
@@ -5189,7 +5225,7 @@
       </c>
     </row>
     <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="82" t="s">
+      <c r="B53" s="93" t="s">
         <v>59</v>
       </c>
       <c r="C53" s="14" t="s">
@@ -5255,7 +5291,7 @@
       </c>
     </row>
     <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="82"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="14" t="s">
         <v>64</v>
       </c>
@@ -5380,11 +5416,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
@@ -5393,6 +5424,11 @@
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B45:B48"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L55">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="NA">

</xml_diff>

<commit_message>
Add some docurmentation and update the ISA excel
</commit_message>
<xml_diff>
--- a/docs/assets/other/ISA.xlsx
+++ b/docs/assets/other/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathias.capdet\AppData\Local\_code\c-sharp\cpu-simple\docs\assets\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2B7DF9-728E-4E4E-AE72-B317323B6C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026FFA6F-8CC6-4AEF-80F9-FF2B53BA4A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="19400" windowHeight="11600" xr2:uid="{627EB5EA-0153-408A-A67D-CE8ACF8A023B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1437,6 +1437,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1472,24 +1490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1877,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D0906C-64AD-4CED-BC8D-ADC11E443218}">
   <dimension ref="B1:AK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1907,16 +1907,16 @@
   <sheetData>
     <row r="1" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="83"/>
+      <c r="D2" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="89"/>
     </row>
     <row r="3" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
@@ -1982,21 +1982,21 @@
       </c>
       <c r="X3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(W4:W55,1),"0"), TEXT(COUNTIF(W4:W55,"&gt;=0"),"0"))</f>
-        <v>48/51</v>
+        <v>51/51</v>
       </c>
       <c r="Z3" s="72" t="s">
         <v>158</v>
       </c>
       <c r="AA3" s="80" t="str">
         <f>_xlfn.TEXTJOIN("/",TRUE,TEXT(COUNTIF(Z4:Z55,1),"0"), TEXT(COUNTIF(Z4:Z55,"&gt;=0"),"0"))</f>
-        <v>48/51</v>
+        <v>51/51</v>
       </c>
       <c r="AK3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="91" t="s">
         <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
@@ -2065,7 +2065,7 @@
       </c>
     </row>
     <row r="5" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="86"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2132,7 @@
       </c>
     </row>
     <row r="6" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="86"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
@@ -2199,7 +2199,7 @@
       </c>
     </row>
     <row r="7" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="86"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
     </row>
     <row r="8" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="86"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="14" t="s">
         <v>15</v>
       </c>
@@ -2333,7 +2333,7 @@
       </c>
     </row>
     <row r="9" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="86"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
@@ -2400,7 +2400,7 @@
       </c>
     </row>
     <row r="10" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="86"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="14" t="s">
         <v>167</v>
       </c>
@@ -2457,17 +2457,17 @@
         <v>50</v>
       </c>
       <c r="W10" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="87"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="14" t="s">
         <v>168</v>
       </c>
@@ -2524,17 +2524,17 @@
         <v>49</v>
       </c>
       <c r="W11" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="94" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2603,7 +2603,7 @@
       </c>
     </row>
     <row r="13" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="89"/>
+      <c r="B13" s="95"/>
       <c r="C13" s="14" t="s">
         <v>169</v>
       </c>
@@ -2657,17 +2657,17 @@
       <c r="S13" s="77"/>
       <c r="T13" s="12"/>
       <c r="W13" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="89"/>
+      <c r="B14" s="95"/>
       <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
@@ -2731,7 +2731,7 @@
       </c>
     </row>
     <row r="15" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="89"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
@@ -2795,7 +2795,7 @@
       </c>
     </row>
     <row r="16" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="89"/>
+      <c r="B16" s="95"/>
       <c r="C16" s="14" t="s">
         <v>10</v>
       </c>
@@ -2859,7 +2859,7 @@
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="89"/>
+      <c r="B17" s="95"/>
       <c r="C17" s="14" t="s">
         <v>9</v>
       </c>
@@ -2923,7 +2923,7 @@
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="89"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="14" t="s">
         <v>6</v>
       </c>
@@ -2989,7 +2989,7 @@
       </c>
     </row>
     <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="90"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="14" t="s">
         <v>5</v>
       </c>
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="90" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -3121,7 +3121,7 @@
       </c>
     </row>
     <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="84"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="14" t="s">
         <v>155</v>
       </c>
@@ -3185,7 +3185,7 @@
       </c>
     </row>
     <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="84"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="14" t="s">
         <v>21</v>
       </c>
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="23" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="84"/>
+      <c r="B23" s="90"/>
       <c r="C23" s="14" t="s">
         <v>157</v>
       </c>
@@ -3313,7 +3313,7 @@
       </c>
     </row>
     <row r="24" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="97" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -3379,7 +3379,7 @@
       </c>
     </row>
     <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="92"/>
+      <c r="B25" s="98"/>
       <c r="C25" s="14" t="s">
         <v>154</v>
       </c>
@@ -3443,7 +3443,7 @@
       </c>
     </row>
     <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="81" t="s">
         <v>160</v>
       </c>
       <c r="C26" s="14" t="s">
@@ -3511,7 +3511,7 @@
       </c>
     </row>
     <row r="27" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="93"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="14" t="s">
         <v>162</v>
       </c>
@@ -3643,7 +3643,7 @@
       </c>
     </row>
     <row r="29" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="83" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
@@ -3711,7 +3711,7 @@
       </c>
     </row>
     <row r="30" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="95"/>
+      <c r="B30" s="83"/>
       <c r="C30" s="14" t="s">
         <v>35</v>
       </c>
@@ -3777,7 +3777,7 @@
       </c>
     </row>
     <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="95"/>
+      <c r="B31" s="83"/>
       <c r="C31" s="14" t="s">
         <v>36</v>
       </c>
@@ -3843,7 +3843,7 @@
       </c>
     </row>
     <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="95"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="14" t="s">
         <v>37</v>
       </c>
@@ -3909,7 +3909,7 @@
       </c>
     </row>
     <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="96" t="s">
+      <c r="B33" s="84" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -3977,7 +3977,7 @@
       </c>
     </row>
     <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="96"/>
+      <c r="B34" s="84"/>
       <c r="C34" s="14" t="s">
         <v>32</v>
       </c>
@@ -4043,7 +4043,7 @@
       </c>
     </row>
     <row r="35" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="97" t="s">
+      <c r="B35" s="85" t="s">
         <v>62</v>
       </c>
       <c r="C35" s="14" t="s">
@@ -4111,7 +4111,7 @@
       </c>
     </row>
     <row r="36" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="97"/>
+      <c r="B36" s="85"/>
       <c r="C36" s="14" t="s">
         <v>30</v>
       </c>
@@ -4177,7 +4177,7 @@
       </c>
     </row>
     <row r="37" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="97"/>
+      <c r="B37" s="85"/>
       <c r="C37" s="14" t="s">
         <v>60</v>
       </c>
@@ -4243,7 +4243,7 @@
       </c>
     </row>
     <row r="38" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="97"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="14" t="s">
         <v>61</v>
       </c>
@@ -4309,7 +4309,7 @@
       </c>
     </row>
     <row r="39" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="86" t="s">
         <v>57</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -4377,7 +4377,7 @@
       </c>
     </row>
     <row r="40" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="98"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="14" t="s">
         <v>41</v>
       </c>
@@ -4443,7 +4443,7 @@
       </c>
     </row>
     <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="98"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="14" t="s">
         <v>42</v>
       </c>
@@ -4507,7 +4507,7 @@
       </c>
     </row>
     <row r="42" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="98"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="14" t="s">
         <v>43</v>
       </c>
@@ -4705,7 +4705,7 @@
       </c>
     </row>
     <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="95" t="s">
+      <c r="B45" s="83" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="14" t="s">
@@ -4771,7 +4771,7 @@
       </c>
     </row>
     <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="95"/>
+      <c r="B46" s="83"/>
       <c r="C46" s="14" t="s">
         <v>45</v>
       </c>
@@ -4835,7 +4835,7 @@
       </c>
     </row>
     <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="95"/>
+      <c r="B47" s="83"/>
       <c r="C47" s="14" t="s">
         <v>46</v>
       </c>
@@ -4899,7 +4899,7 @@
       </c>
     </row>
     <row r="48" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="95"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="14" t="s">
         <v>47</v>
       </c>
@@ -5095,7 +5095,7 @@
       </c>
     </row>
     <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="94" t="s">
+      <c r="B51" s="82" t="s">
         <v>65</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -5161,7 +5161,7 @@
       </c>
     </row>
     <row r="52" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="94"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="14" t="s">
         <v>39</v>
       </c>
@@ -5225,7 +5225,7 @@
       </c>
     </row>
     <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="93" t="s">
+      <c r="B53" s="81" t="s">
         <v>59</v>
       </c>
       <c r="C53" s="14" t="s">
@@ -5291,7 +5291,7 @@
       </c>
     </row>
     <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="93"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="14" t="s">
         <v>64</v>
       </c>
@@ -5416,6 +5416,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
@@ -5424,11 +5429,6 @@
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B45:B48"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L55">
     <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="NA">

</xml_diff>